<commit_message>
Print error messages and update tp and template-es
</commit_message>
<xml_diff>
--- a/testdata/template-es.xlsx
+++ b/testdata/template-es.xlsx
@@ -891,8 +891,8 @@
   </sheetPr>
   <dimension ref="A1:U12"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100">
-      <selection activeCell="O4" activeCellId="0" pane="topLeft" sqref="O4"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="J1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100">
+      <selection activeCell="O2" activeCellId="0" pane="topLeft" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <cols>

</xml_diff>